<commit_message>
last update on pert & gantt
</commit_message>
<xml_diff>
--- a/Documents-Gestion/PERT-GANTT/PERT & GANTT Final/Pert & GANTT SAE.xlsx
+++ b/Documents-Gestion/PERT-GANTT/PERT & GANTT Final/Pert & GANTT SAE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\Documents\Projets\SAE.3\AR-tistic\Documents-Gestion\PERT-GANTT\PERT &amp; GANTT Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913A603E-906D-437D-B0E7-1AF4F6FC1CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F58D3E-17A7-42EC-85B9-0CE5D2F1FE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{9B79E3AB-03E4-4F1E-A9FE-3328D6A52758}"/>
   </bookViews>
@@ -243,7 +243,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,11 +277,6 @@
       <color theme="7"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
-      <name val="Oswald"/>
     </font>
     <font>
       <sz val="11"/>
@@ -529,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -552,6 +547,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -564,26 +562,8 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -599,91 +579,88 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="14" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -810,10 +787,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>10</c:v>
@@ -828,7 +805,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>25</c:v>
@@ -837,7 +814,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>10</c:v>
@@ -849,10 +826,10 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>30</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>50</c:v>
@@ -2867,7 +2844,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E9056201-808B-4444-A3F5-EF8F7DF370FF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2878,7 +2855,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9283290" cy="6055032"/>
+    <xdr:ext cx="9295140" cy="6070810"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1">
@@ -3247,8 +3224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC2240F-CDED-4B55-868B-4AC221664F00}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="42" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="93" zoomScaleNormal="42" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3257,931 +3234,931 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="46" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="47"/>
-      <c r="I1" s="40" t="s">
+      <c r="H1" s="40"/>
+      <c r="I1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="38" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="43"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="42">
         <v>5</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51">
+      <c r="D3" s="43"/>
+      <c r="E3" s="44">
         <v>0</v>
       </c>
-      <c r="F3" s="50">
+      <c r="F3" s="43">
         <v>5</v>
       </c>
-      <c r="G3" s="50">
+      <c r="G3" s="43">
         <f t="shared" ref="G3:G24" si="0">H3-C3</f>
         <v>0</v>
       </c>
-      <c r="H3" s="50">
+      <c r="H3" s="43">
         <f>MIN(G4)</f>
         <v>5</v>
       </c>
-      <c r="I3" s="52">
+      <c r="I3" s="45">
         <f t="shared" ref="I3:I24" si="1">H3-F3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="53">
+      <c r="J3" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="42">
         <v>7</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="43">
         <f>F3</f>
         <v>5</v>
       </c>
-      <c r="F4" s="50">
+      <c r="F4" s="43">
         <f>E4+C4</f>
         <v>12</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="43">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H4" s="50">
+      <c r="H4" s="43">
         <f>MIN(G5)</f>
         <v>12</v>
       </c>
-      <c r="I4" s="52">
+      <c r="I4" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J4" s="53">
+      <c r="J4" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="42">
         <v>13</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="50">
+      <c r="E5" s="43">
         <f>F4</f>
         <v>12</v>
       </c>
-      <c r="F5" s="50">
+      <c r="F5" s="43">
         <f t="shared" ref="F5:F26" si="2">E5+C5</f>
         <v>25</v>
       </c>
-      <c r="G5" s="50">
+      <c r="G5" s="43">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H5" s="50">
+      <c r="H5" s="43">
         <f>MIN(G6,G7,G8)</f>
         <v>25</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J5" s="53">
+      <c r="J5" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="42">
         <v>15</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="43">
         <f>F5</f>
         <v>25</v>
       </c>
-      <c r="F6" s="50">
+      <c r="F6" s="43">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="G6" s="50">
+      <c r="G6" s="43">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H6" s="50">
+      <c r="H6" s="43">
         <f>MIN(G8)</f>
         <v>40</v>
       </c>
-      <c r="I6" s="52">
+      <c r="I6" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J6" s="53">
+      <c r="J6" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="42">
         <v>10</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="43">
         <f>MAX(F5,F8)</f>
         <v>50</v>
       </c>
-      <c r="F7" s="50">
+      <c r="F7" s="43">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="G7" s="50">
+      <c r="G7" s="43">
         <f t="shared" si="0"/>
-        <v>220</v>
-      </c>
-      <c r="H7" s="50">
+        <v>175</v>
+      </c>
+      <c r="H7" s="43">
         <f>MIN(F25)</f>
-        <v>230</v>
-      </c>
-      <c r="I7" s="52">
+        <v>185</v>
+      </c>
+      <c r="I7" s="45">
         <f t="shared" si="1"/>
-        <v>170</v>
-      </c>
-      <c r="J7" s="53">
+        <v>125</v>
+      </c>
+      <c r="J7" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="42">
         <v>10</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="43">
         <f>MAX(F5,F6)</f>
         <v>40</v>
       </c>
-      <c r="F8" s="50">
+      <c r="F8" s="43">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="G8" s="50">
+      <c r="G8" s="43">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="H8" s="50">
+      <c r="H8" s="43">
         <f>MIN(G10,G16,G7,G10,G11,G20)</f>
         <v>50</v>
       </c>
-      <c r="I8" s="52">
+      <c r="I8" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="53">
+      <c r="J8" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="42">
         <v>10</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="44">
         <f>MAX(F10,F11)</f>
-        <v>60</v>
-      </c>
-      <c r="F9" s="50">
+        <v>65</v>
+      </c>
+      <c r="F9" s="43">
         <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="G9" s="50">
+        <v>75</v>
+      </c>
+      <c r="G9" s="43">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="H9" s="43">
+        <f>MIN(G14)</f>
+        <v>75</v>
+      </c>
+      <c r="I9" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="42">
+        <v>5</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="44">
+        <f>MAX(F8)</f>
+        <v>50</v>
+      </c>
+      <c r="F10" s="43">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="G10" s="43">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H9" s="50">
-        <f>MIN(G14)</f>
-        <v>70</v>
-      </c>
-      <c r="I9" s="52">
+      <c r="H10" s="43">
+        <f>MIN(G13,G9)</f>
+        <v>65</v>
+      </c>
+      <c r="I10" s="45">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J10" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="42">
+        <v>15</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="44">
+        <f>MAX(F8)</f>
+        <v>50</v>
+      </c>
+      <c r="F11" s="43">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="G11" s="43">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="H11" s="43">
+        <f>MIN(G13,G9)</f>
+        <v>65</v>
+      </c>
+      <c r="I11" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J9" s="53">
+      <c r="J11" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="49">
-        <v>5</v>
-      </c>
-      <c r="D10" s="49" t="s">
+    <row r="12" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="42">
+        <v>15</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="44">
+        <f>MAX(F14)</f>
+        <v>100</v>
+      </c>
+      <c r="F12" s="43">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="G12" s="43">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H12" s="43">
+        <f>MIN(G13)</f>
+        <v>115</v>
+      </c>
+      <c r="I12" s="45">
+        <f>H12-F12</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="42">
+        <v>10</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="44">
+        <f>MAX(F10,F11,F12)</f>
+        <v>115</v>
+      </c>
+      <c r="F13" s="43">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+      <c r="G13" s="43">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="H13" s="43">
+        <f>MIN(G21,G22,G23)</f>
+        <v>125</v>
+      </c>
+      <c r="I13" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="42">
+        <v>25</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="44">
+        <f>MAX(F9)</f>
+        <v>75</v>
+      </c>
+      <c r="F14" s="43">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G14" s="43">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="H14" s="43">
+        <f>MIN(G15,G21,G22,G23,G12)</f>
+        <v>100</v>
+      </c>
+      <c r="I14" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="42">
+        <v>18</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="44">
+        <f>MAX(F14)</f>
+        <v>100</v>
+      </c>
+      <c r="F15" s="43">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="G15" s="43">
+        <f t="shared" si="0"/>
+        <v>167</v>
+      </c>
+      <c r="H15" s="43">
+        <f>MIN(F25)</f>
+        <v>185</v>
+      </c>
+      <c r="I15" s="45">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="J15" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="42">
+        <v>7</v>
+      </c>
+      <c r="D16" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E16" s="43">
         <f>MAX(F8)</f>
         <v>50</v>
       </c>
-      <c r="F10" s="50">
+      <c r="F16" s="43">
         <f t="shared" si="2"/>
-        <v>55</v>
-      </c>
-      <c r="G10" s="50">
+        <v>57</v>
+      </c>
+      <c r="G16" s="43">
         <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="H10" s="50">
-        <f>MIN(G13,G9)</f>
-        <v>60</v>
-      </c>
-      <c r="I10" s="52">
+        <v>63</v>
+      </c>
+      <c r="H16" s="43">
+        <f>MIN(G17)</f>
+        <v>70</v>
+      </c>
+      <c r="I16" s="45">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="J10" s="53">
+        <v>13</v>
+      </c>
+      <c r="J16" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="49" t="s">
+    <row r="17" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="42">
         <v>30</v>
       </c>
-      <c r="C11" s="49">
-        <v>10</v>
-      </c>
-      <c r="D11" s="49" t="s">
+      <c r="D17" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="44">
+        <f>MAX(F16)</f>
+        <v>57</v>
+      </c>
+      <c r="F17" s="43">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="G17" s="43">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="H17" s="43">
+        <f>MIN(G18)</f>
+        <v>100</v>
+      </c>
+      <c r="I17" s="45">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J17" s="46">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="42">
+        <v>25</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="44">
+        <f>MAX(F17)</f>
+        <v>87</v>
+      </c>
+      <c r="F18" s="43">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="G18" s="43">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H18" s="43">
+        <f>MIN(G19)</f>
+        <v>125</v>
+      </c>
+      <c r="I18" s="45">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J18" s="46">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="19">
+        <v>50</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="15">
+        <f>MAX(F18)</f>
+        <v>112</v>
+      </c>
+      <c r="F19" s="16">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+      <c r="G19" s="16">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="H19" s="16">
+        <f>MIN(G24)</f>
+        <v>175</v>
+      </c>
+      <c r="I19" s="17">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J19" s="18">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="19">
+        <v>50</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="51">
+      <c r="E20" s="15">
         <f>MAX(F8)</f>
         <v>50</v>
       </c>
-      <c r="F11" s="50">
+      <c r="F20" s="16">
         <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="G11" s="50">
+        <v>100</v>
+      </c>
+      <c r="G20" s="16">
         <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="H20" s="16">
+        <f>MIN(G24)</f>
+        <v>175</v>
+      </c>
+      <c r="I20" s="17">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="J20" s="18">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="50">
-        <f>MIN(G13,G9)</f>
-        <v>60</v>
-      </c>
-      <c r="I11" s="52">
+      <c r="B21" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="19">
+        <v>10</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="15">
+        <f>MAX(F14,F13)</f>
+        <v>125</v>
+      </c>
+      <c r="F21" s="16">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="G21" s="16">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="H21" s="16">
+        <f>MIN(G24)</f>
+        <v>175</v>
+      </c>
+      <c r="I21" s="17">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J21" s="18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="19">
+        <v>50</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="15">
+        <f>MAX(F14,F13)</f>
+        <v>125</v>
+      </c>
+      <c r="F22" s="16">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="G22" s="16">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="H22" s="16">
+        <f>MIN(G24)</f>
+        <v>175</v>
+      </c>
+      <c r="I22" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="49">
-        <v>30</v>
-      </c>
-      <c r="D12" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="51">
-        <f>MAX(F14)</f>
-        <v>95</v>
-      </c>
-      <c r="F12" s="50">
+      <c r="J22" s="18">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="19">
+        <v>35</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="15">
+        <f>MAX(F14,F13)</f>
+        <v>125</v>
+      </c>
+      <c r="F23" s="16">
         <f t="shared" si="2"/>
-        <v>125</v>
-      </c>
-      <c r="G12" s="50">
+        <v>160</v>
+      </c>
+      <c r="G23" s="16">
         <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-      <c r="H12" s="50">
-        <f>MIN(G13)</f>
-        <v>125</v>
-      </c>
-      <c r="I12" s="52">
-        <f>H12-F12</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="49">
+        <v>140</v>
+      </c>
+      <c r="H23" s="16">
+        <f>MIN(G24)</f>
+        <v>175</v>
+      </c>
+      <c r="I23" s="17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J23" s="18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="111" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="21">
         <v>10</v>
       </c>
-      <c r="D13" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="51">
-        <f>MAX(F10,F11,F12)</f>
-        <v>125</v>
-      </c>
-      <c r="F13" s="50">
+      <c r="D24" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="22">
+        <f>MAX(F19,F20,F21,F22,F23)</f>
+        <v>175</v>
+      </c>
+      <c r="F24" s="23">
         <f t="shared" si="2"/>
-        <v>135</v>
-      </c>
-      <c r="G13" s="50">
+        <v>185</v>
+      </c>
+      <c r="G24" s="23">
         <f t="shared" si="0"/>
-        <v>125</v>
-      </c>
-      <c r="H13" s="50">
-        <f>MIN(G21,G22,G23)</f>
-        <v>135</v>
-      </c>
-      <c r="I13" s="52">
+        <v>175</v>
+      </c>
+      <c r="H24" s="23">
+        <f>MIN(G25)</f>
+        <v>185</v>
+      </c>
+      <c r="I24" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="49">
-        <v>25</v>
-      </c>
-      <c r="D14" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="51">
-        <f>MAX(F9)</f>
-        <v>70</v>
-      </c>
-      <c r="F14" s="50">
-        <f t="shared" si="2"/>
-        <v>95</v>
-      </c>
-      <c r="G14" s="50">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="H14" s="50">
-        <f>MIN(G15,G21,G22,G23,G12)</f>
-        <v>95</v>
-      </c>
-      <c r="I14" s="52">
-        <f t="shared" si="1"/>
+      <c r="J24" s="25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="27">
         <v>0</v>
       </c>
-      <c r="J14" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="49">
-        <v>18</v>
-      </c>
-      <c r="D15" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="51">
-        <f>MAX(F14)</f>
-        <v>95</v>
-      </c>
-      <c r="F15" s="50">
-        <f t="shared" si="2"/>
-        <v>113</v>
-      </c>
-      <c r="G15" s="50">
-        <f t="shared" si="0"/>
-        <v>212</v>
-      </c>
-      <c r="H15" s="50">
-        <f>MIN(F25)</f>
-        <v>230</v>
-      </c>
-      <c r="I15" s="52">
-        <f t="shared" si="1"/>
-        <v>117</v>
-      </c>
-      <c r="J15" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="49">
-        <v>7</v>
-      </c>
-      <c r="D16" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="50">
-        <f>MAX(F8)</f>
-        <v>50</v>
-      </c>
-      <c r="F16" s="50">
-        <f t="shared" si="2"/>
+      <c r="D25" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="50">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="H16" s="50">
-        <f>MIN(G17)</f>
-        <v>95</v>
-      </c>
-      <c r="I16" s="52">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="J16" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="49">
-        <v>15</v>
-      </c>
-      <c r="D17" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="51">
-        <f>MAX(F16)</f>
-        <v>57</v>
-      </c>
-      <c r="F17" s="50">
-        <f t="shared" si="2"/>
-        <v>72</v>
-      </c>
-      <c r="G17" s="50">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-      <c r="H17" s="50">
-        <f>MIN(G18)</f>
-        <v>110</v>
-      </c>
-      <c r="I17" s="52">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="J17" s="53">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="49">
-        <v>25</v>
-      </c>
-      <c r="D18" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="51">
-        <f>MAX(F17)</f>
-        <v>72</v>
-      </c>
-      <c r="F18" s="50">
-        <f t="shared" si="2"/>
-        <v>97</v>
-      </c>
-      <c r="G18" s="50">
-        <f t="shared" si="0"/>
-        <v>110</v>
-      </c>
-      <c r="H18" s="50">
-        <f>MIN(G19)</f>
-        <v>135</v>
-      </c>
-      <c r="I18" s="52">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="J18" s="53">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="25">
-        <v>50</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="20">
-        <f>MAX(F18)</f>
-        <v>97</v>
-      </c>
-      <c r="F19" s="50">
-        <f t="shared" si="2"/>
-        <v>147</v>
-      </c>
-      <c r="G19" s="21">
-        <f t="shared" si="0"/>
-        <v>135</v>
-      </c>
-      <c r="H19" s="21">
-        <f>MIN(G24)</f>
+      <c r="E25" s="28">
+        <f>MAX(F24)</f>
         <v>185</v>
       </c>
-      <c r="I19" s="22">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="J19" s="23">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="25">
-        <v>90</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="20">
-        <f>MAX(F8)</f>
-        <v>50</v>
-      </c>
-      <c r="F20" s="50">
-        <f t="shared" si="2"/>
-        <v>140</v>
-      </c>
-      <c r="G20" s="21">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-      <c r="H20" s="21">
-        <f>MIN(G24)</f>
-        <v>185</v>
-      </c>
-      <c r="I20" s="22">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="J20" s="23">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="25">
-        <v>10</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="20">
-        <f>MAX(F14,F13)</f>
-        <v>135</v>
-      </c>
-      <c r="F21" s="50">
-        <f t="shared" si="2"/>
-        <v>145</v>
-      </c>
-      <c r="G21" s="21">
-        <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-      <c r="H21" s="21">
-        <f>MIN(G24)</f>
-        <v>185</v>
-      </c>
-      <c r="I21" s="22">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="J21" s="23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="25">
-        <v>50</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="20">
-        <f>MAX(F14,F13)</f>
-        <v>135</v>
-      </c>
-      <c r="F22" s="50">
+      <c r="F25" s="29">
         <f t="shared" si="2"/>
         <v>185</v>
       </c>
-      <c r="G22" s="21">
-        <f t="shared" si="0"/>
-        <v>135</v>
-      </c>
-      <c r="H22" s="21">
-        <f>MIN(G24)</f>
+      <c r="G25" s="29">
+        <f>H25-C25</f>
         <v>185</v>
       </c>
-      <c r="I22" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="23">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="25">
-        <v>35</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="20">
-        <f>MAX(F14,F13)</f>
-        <v>135</v>
-      </c>
-      <c r="F23" s="50">
-        <f t="shared" si="2"/>
-        <v>170</v>
-      </c>
-      <c r="G23" s="21">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="H23" s="21">
-        <f>MIN(G24)</f>
+      <c r="H25" s="29">
+        <f>F25</f>
         <v>185</v>
       </c>
-      <c r="I23" s="22">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="J23" s="23">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="111" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="27">
-        <v>30</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="28">
-        <f>MAX(F19,F20,F21,F22,F23)</f>
-        <v>185</v>
-      </c>
-      <c r="F24" s="50">
-        <f t="shared" si="2"/>
-        <v>215</v>
-      </c>
-      <c r="G24" s="29">
-        <f t="shared" si="0"/>
-        <v>185</v>
-      </c>
-      <c r="H24" s="29">
-        <f>MIN(G25)</f>
-        <v>215</v>
-      </c>
-      <c r="I24" s="30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="31">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="33">
-        <v>15</v>
-      </c>
-      <c r="D25" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="34">
-        <f>MAX(F24)</f>
-        <v>215</v>
-      </c>
-      <c r="F25" s="50">
-        <f t="shared" si="2"/>
-        <v>230</v>
-      </c>
-      <c r="G25" s="35">
-        <f>H25-C25</f>
-        <v>215</v>
-      </c>
-      <c r="H25" s="35">
-        <f>F25</f>
-        <v>230</v>
-      </c>
-      <c r="I25" s="36">
+      <c r="I25" s="30">
         <f>H25-F25</f>
         <v>0</v>
       </c>
-      <c r="J25" s="37">
+      <c r="J25" s="31">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="42">
         <v>50</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15">
+      <c r="D26" s="44"/>
+      <c r="E26" s="44">
         <v>0</v>
       </c>
-      <c r="F26" s="50">
+      <c r="F26" s="43">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="43">
         <f>H26-C26</f>
-        <v>180</v>
-      </c>
-      <c r="H26" s="16">
+        <v>135</v>
+      </c>
+      <c r="H26" s="43">
         <f>F25</f>
-        <v>230</v>
-      </c>
-      <c r="I26" s="17">
+        <v>185</v>
+      </c>
+      <c r="I26" s="45">
         <f>H26-F26</f>
-        <v>180</v>
-      </c>
-      <c r="J26" s="18">
+        <v>135</v>
+      </c>
+      <c r="J26" s="46">
         <v>1</v>
       </c>
     </row>
@@ -4205,8 +4182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49CB231-24FF-40E3-A85B-F6B59BCCB429}">
   <dimension ref="A1:AV25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="35" workbookViewId="0">
-      <selection activeCell="AA23" sqref="AA23"/>
+    <sheetView zoomScale="69" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4222,7 +4199,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:48" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:48" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -4233,7 +4210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:48" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:48" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -4255,7 +4232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:48" ht="91.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:48" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -4288,7 +4265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:48" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:48" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -4310,7 +4287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:48" ht="69" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:48" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -4321,7 +4298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:48" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:48" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -4332,7 +4309,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:48" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:48" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
@@ -4343,7 +4320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:48" ht="46.2" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:48" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -4355,7 +4332,7 @@
       </c>
       <c r="AV13" s="13"/>
     </row>
-    <row r="14" spans="1:48" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:48" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -4399,7 +4376,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>47</v>
       </c>
@@ -4410,7 +4387,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="69" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>49</v>
       </c>
@@ -4421,7 +4398,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>51</v>
       </c>
@@ -4432,7 +4409,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>54</v>
       </c>
@@ -4443,7 +4420,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>56</v>
       </c>

</xml_diff>